<commit_message>
Update Leaves and delete module notification
</commit_message>
<xml_diff>
--- a/uploads/optiflow.xlsx
+++ b/uploads/optiflow.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
   <si>
     <t>Horodateur</t>
   </si>
@@ -158,6 +158,39 @@
   </si>
   <si>
     <t xml:space="preserve"> j teb fdopgpre</t>
+  </si>
+  <si>
+    <t>05/04/2024 08:48:16</t>
+  </si>
+  <si>
+    <t>trabelsi.ahmed.1@esprit.tn</t>
+  </si>
+  <si>
+    <t>ahmed</t>
+  </si>
+  <si>
+    <t>ca va</t>
+  </si>
+  <si>
+    <t>oui</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
+  <si>
+    <t>23/04/2024 22:11:13</t>
+  </si>
+  <si>
+    <t>aymen.nefzi@esprit.tn</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>aaaa</t>
   </si>
 </sst>
 </file>
@@ -534,7 +567,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -695,6 +728,70 @@
       </c>
       <c r="J5" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>